<commit_message>
Added figure of associations to chapter 3, added to the introduction of chapter 3.
</commit_message>
<xml_diff>
--- a/Dissertation Chapters/Chapter 3/PRESS_Chapter3_tables.xlsx
+++ b/Dissertation Chapters/Chapter 3/PRESS_Chapter3_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mollyec/Documents/GitHub/Developmental-Obesity/Dissertation Chapters/Chapter 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A19CA6-D959-E540-AE6A-9C30FF3E20F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1541570C-ED72-4E4F-B658-B4666D0044C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38120" yWindow="1080" windowWidth="36180" windowHeight="16400" activeTab="4" xr2:uid="{5531AC36-D13B-7248-9642-950AE3589228}"/>
+    <workbookView xWindow="-35760" yWindow="1560" windowWidth="28800" windowHeight="16360" activeTab="5" xr2:uid="{5531AC36-D13B-7248-9642-950AE3589228}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1, Base Demographics" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Demo_tri2_weekend" sheetId="4" r:id="rId4"/>
     <sheet name="Demo_tri3_weekday" sheetId="6" r:id="rId5"/>
     <sheet name="Demo_tri3_weekend" sheetId="7" r:id="rId6"/>
-    <sheet name="Shift averages" sheetId="5" r:id="rId7"/>
+    <sheet name="unadjusted models_BW" sheetId="8" r:id="rId7"/>
+    <sheet name="Shift averages" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,8 +42,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="719">
   <si>
     <t>Maternal Characteristics</t>
   </si>
@@ -1187,9 +1225,6 @@
     <t>Table 1: Bivariate analysis, Trimester 3 exposure data</t>
   </si>
   <si>
-    <t>n=</t>
-  </si>
-  <si>
     <t xml:space="preserve">fasting midpoint weekday </t>
   </si>
   <si>
@@ -2151,6 +2186,57 @@
   </si>
   <si>
     <t>11.1 (2.52)</t>
+  </si>
+  <si>
+    <t>summary table of all significant effects</t>
+  </si>
+  <si>
+    <t>calculate variance in weekend values - determine if the measure is noise (levene/sd/se)</t>
+  </si>
+  <si>
+    <t>rrun baase model - summarize AIC/BICC/R2 which of 16 variables explains the most variannce in ogtt and bw</t>
+  </si>
+  <si>
+    <t>model%&gt;%glance%&gt;%kable</t>
+  </si>
+  <si>
+    <t>load broom first</t>
+  </si>
+  <si>
+    <t>unadjusted model</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Model 4</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>Beta (95% CI)</t>
+  </si>
+  <si>
+    <t>*p value is from a Wald's test</t>
+  </si>
+  <si>
+    <t>unadj: infant birth weight (g) ~ first eat</t>
+  </si>
+  <si>
+    <t>TRIMESTER 2</t>
+  </si>
+  <si>
+    <t>Table 6: Infant birth weight based on timing of first meal</t>
+  </si>
+  <si>
+    <t>n=63</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2229,8 +2315,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2289,6 +2390,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2448,7 +2555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2608,26 +2715,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2641,14 +2733,31 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2665,6 +2774,68 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>4</v>
+    <v>8</v>
+    <v>7</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2977,10 +3148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="72"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3585,8 +3756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8203B5-6C52-824B-A87C-392F3FBA75E7}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I15" sqref="F15:I16"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4749,8 +4920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D53AF2D-22C6-784B-BF77-C2DEAEA75735}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4761,14 +4932,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="52" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -4782,7 +4953,7 @@
         <v>225</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F2" s="55" t="s">
         <v>227</v>
@@ -4830,10 +5001,10 @@
         <v>286</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4849,11 +5020,11 @@
       <c r="D6" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="E6" s="73" t="s">
-        <v>384</v>
+      <c r="E6" s="68" t="s">
+        <v>383</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4869,11 +5040,11 @@
       <c r="D7" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="E7" s="73" t="s">
-        <v>385</v>
+      <c r="E7" s="68" t="s">
+        <v>384</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -4889,11 +5060,11 @@
       <c r="D8" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="E8" s="73" t="s">
-        <v>386</v>
+      <c r="E8" s="68" t="s">
+        <v>385</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4909,11 +5080,11 @@
       <c r="D9" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="E9" s="73" t="s">
-        <v>387</v>
+      <c r="E9" s="68" t="s">
+        <v>386</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4929,11 +5100,11 @@
       <c r="D10" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="E10" s="73" t="s">
-        <v>388</v>
+      <c r="E10" s="68" t="s">
+        <v>387</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4959,10 +5130,10 @@
         <v>282</v>
       </c>
       <c r="B12" s="37"/>
-      <c r="C12" s="67"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="37"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -4977,11 +5148,11 @@
       <c r="D13" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="73" t="s">
-        <v>383</v>
+      <c r="E13" s="68" t="s">
+        <v>382</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -4997,22 +5168,22 @@
       <c r="D14" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="E14" s="73" t="s">
-        <v>389</v>
+      <c r="E14" s="68" t="s">
+        <v>388</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="64" t="s">
         <v>140</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="62">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D15" s="71">
+      <c r="D15" s="66">
         <v>0.04</v>
       </c>
       <c r="E15" s="62">
@@ -5045,11 +5216,11 @@
       <c r="D17" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="E17" s="73" t="s">
-        <v>390</v>
+      <c r="E17" s="68" t="s">
+        <v>389</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5065,11 +5236,11 @@
       <c r="D18" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E18" s="73" t="s">
-        <v>391</v>
+      <c r="E18" s="68" t="s">
+        <v>390</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5113,11 +5284,11 @@
       <c r="D21" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="E21" s="73" t="s">
-        <v>392</v>
+      <c r="E21" s="68" t="s">
+        <v>391</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5133,11 +5304,11 @@
       <c r="D22" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="E22" s="73" t="s">
-        <v>393</v>
+      <c r="E22" s="68" t="s">
+        <v>392</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5153,11 +5324,11 @@
       <c r="D23" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="E23" s="73" t="s">
-        <v>394</v>
+      <c r="E23" s="68" t="s">
+        <v>393</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5201,11 +5372,11 @@
       <c r="D26" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="E26" s="73" t="s">
-        <v>395</v>
+      <c r="E26" s="68" t="s">
+        <v>394</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5213,7 +5384,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="13">
-        <v>2422</v>
+        <v>22</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>255</v>
@@ -5221,11 +5392,11 @@
       <c r="D27" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="E27" s="73" t="s">
-        <v>383</v>
+      <c r="E27" s="68" t="s">
+        <v>382</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5238,14 +5409,14 @@
       <c r="C28" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="E28" s="73" t="s">
-        <v>396</v>
+      <c r="E28" s="68" t="s">
+        <v>395</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5261,11 +5432,11 @@
       <c r="D29" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="E29" s="73" t="s">
-        <v>383</v>
+      <c r="E29" s="68" t="s">
+        <v>382</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5309,11 +5480,11 @@
       <c r="D32" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="E32" s="73" t="s">
-        <v>391</v>
+      <c r="E32" s="68" t="s">
+        <v>390</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5329,11 +5500,11 @@
       <c r="D33" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="E33" s="73" t="s">
-        <v>397</v>
+      <c r="E33" s="68" t="s">
+        <v>396</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5349,11 +5520,11 @@
       <c r="D34" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="E34" s="73" t="s">
-        <v>398</v>
+      <c r="E34" s="68" t="s">
+        <v>397</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5369,11 +5540,11 @@
       <c r="D35" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="E35" s="73" t="s">
-        <v>399</v>
+      <c r="E35" s="68" t="s">
+        <v>398</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5417,11 +5588,11 @@
       <c r="D38" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="E38" s="73" t="s">
-        <v>400</v>
+      <c r="E38" s="68" t="s">
+        <v>399</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -5437,11 +5608,11 @@
       <c r="D39" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="E39" s="73" t="s">
-        <v>401</v>
+      <c r="E39" s="68" t="s">
+        <v>400</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -5457,11 +5628,11 @@
       <c r="D40" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="E40" s="73" t="s">
-        <v>402</v>
+      <c r="E40" s="68" t="s">
+        <v>401</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5472,7 +5643,7 @@
       <c r="C41" s="28">
         <v>0.24</v>
       </c>
-      <c r="D41" s="72">
+      <c r="D41" s="67">
         <v>0.35</v>
       </c>
       <c r="E41" s="28">
@@ -5505,11 +5676,11 @@
       <c r="D43" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="E43" s="73" t="s">
-        <v>391</v>
+      <c r="E43" s="68" t="s">
+        <v>390</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5525,11 +5696,11 @@
       <c r="D44" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="E44" s="73" t="s">
-        <v>397</v>
+      <c r="E44" s="68" t="s">
+        <v>396</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5540,7 +5711,7 @@
       <c r="C45" s="62">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="D45" s="71">
+      <c r="D45" s="66">
         <v>1.2E-2</v>
       </c>
       <c r="E45" s="28">
@@ -5573,11 +5744,11 @@
       <c r="D47" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="E47" s="73" t="s">
-        <v>397</v>
+      <c r="E47" s="68" t="s">
+        <v>396</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5593,11 +5764,11 @@
       <c r="D48" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="E48" s="73" t="s">
-        <v>392</v>
+      <c r="E48" s="68" t="s">
+        <v>391</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5613,11 +5784,11 @@
       <c r="D49" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="E49" s="73" t="s">
-        <v>403</v>
+      <c r="E49" s="68" t="s">
+        <v>402</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5661,11 +5832,11 @@
       <c r="D52" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="E52" s="73" t="s">
-        <v>404</v>
+      <c r="E52" s="68" t="s">
+        <v>403</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5681,11 +5852,11 @@
       <c r="D53" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="E53" s="73" t="s">
-        <v>391</v>
+      <c r="E53" s="68" t="s">
+        <v>390</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5729,11 +5900,11 @@
       <c r="D56" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="E56" s="73" t="s">
-        <v>405</v>
+      <c r="E56" s="68" t="s">
+        <v>404</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5749,11 +5920,11 @@
       <c r="D57" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="E57" s="73" t="s">
-        <v>392</v>
+      <c r="E57" s="68" t="s">
+        <v>391</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5769,11 +5940,11 @@
       <c r="D58" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="E58" s="73" t="s">
-        <v>406</v>
+      <c r="E58" s="68" t="s">
+        <v>405</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5789,11 +5960,11 @@
       <c r="D59" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="E59" s="73" t="s">
-        <v>407</v>
+      <c r="E59" s="68" t="s">
+        <v>406</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5809,11 +5980,11 @@
       <c r="D60" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="E60" s="73" t="s">
-        <v>408</v>
+      <c r="E60" s="68" t="s">
+        <v>407</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5829,11 +6000,11 @@
       <c r="D61" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="E61" s="73" t="s">
-        <v>409</v>
+      <c r="E61" s="68" t="s">
+        <v>408</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5849,11 +6020,11 @@
       <c r="D62" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="E62" s="73" t="s">
-        <v>410</v>
+      <c r="E62" s="68" t="s">
+        <v>409</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5864,7 +6035,7 @@
       <c r="C63" s="28">
         <v>0.62</v>
       </c>
-      <c r="D63" s="70">
+      <c r="D63" s="65">
         <v>0.83</v>
       </c>
       <c r="E63" s="28">
@@ -5897,11 +6068,11 @@
       <c r="D65" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="E65" s="73" t="s">
-        <v>390</v>
+      <c r="E65" s="68" t="s">
+        <v>389</v>
       </c>
       <c r="F65" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5917,11 +6088,11 @@
       <c r="D66" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="E66" s="73" t="s">
-        <v>411</v>
+      <c r="E66" s="68" t="s">
+        <v>410</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5975,11 +6146,11 @@
       <c r="D70" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="E70" s="73" t="s">
-        <v>390</v>
+      <c r="E70" s="68" t="s">
+        <v>389</v>
       </c>
       <c r="F70" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5995,11 +6166,11 @@
       <c r="D71" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="E71" s="73" t="s">
-        <v>401</v>
+      <c r="E71" s="68" t="s">
+        <v>400</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6043,11 +6214,11 @@
       <c r="D74" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="E74" s="73" t="s">
-        <v>412</v>
+      <c r="E74" s="68" t="s">
+        <v>411</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -6063,11 +6234,11 @@
       <c r="D75" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="E75" s="73" t="s">
-        <v>397</v>
+      <c r="E75" s="68" t="s">
+        <v>396</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -6112,10 +6283,10 @@
         <v>317</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -6132,10 +6303,10 @@
         <v>326</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6172,10 +6343,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262C7769-B3A3-CF4D-B17E-7DCF8B138DCE}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6185,17 +6356,17 @@
     <col min="5" max="6" width="13.83203125" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:6" ht="52" x14ac:dyDescent="0.25">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+    </row>
+    <row r="2" spans="1:13" ht="52" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -6213,7 +6384,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="24" t="s">
         <v>246</v>
@@ -6231,7 +6402,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
@@ -6241,7 +6412,7 @@
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -6255,13 +6426,13 @@
         <v>355</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>229</v>
       </c>
@@ -6275,13 +6446,13 @@
         <v>356</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -6295,13 +6466,13 @@
         <v>357</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -6315,13 +6486,13 @@
         <v>360</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -6335,13 +6506,13 @@
         <v>359</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -6355,13 +6526,13 @@
         <v>358</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -6379,17 +6550,17 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>282</v>
       </c>
       <c r="B12" s="37"/>
-      <c r="C12" s="67"/>
+      <c r="C12" s="63"/>
       <c r="D12" s="37"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -6403,13 +6574,17 @@
         <v>355</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>283</v>
       </c>
@@ -6423,21 +6598,27 @@
         <v>289</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+        <v>474</v>
+      </c>
+      <c r="J14" s="76" t="s">
+        <v>702</v>
+      </c>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="64" t="s">
         <v>140</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="62">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D15" s="76">
+      <c r="D15" s="70">
         <v>0.40200000000000002</v>
       </c>
       <c r="E15" s="62">
@@ -6446,8 +6627,14 @@
       <c r="F15" s="28">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="76" t="s">
+        <v>703</v>
+      </c>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+    </row>
+    <row r="16" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6456,8 +6643,14 @@
       <c r="D16" s="12"/>
       <c r="E16" s="60"/>
       <c r="F16" s="60"/>
-    </row>
-    <row r="17" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="76" t="s">
+        <v>704</v>
+      </c>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+    </row>
+    <row r="17" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>247</v>
       </c>
@@ -6471,13 +6664,21 @@
         <v>361</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+      <c r="J17" s="76" t="s">
+        <v>705</v>
+      </c>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76" t="s">
+        <v>706</v>
+      </c>
+      <c r="M17" s="76"/>
+    </row>
+    <row r="18" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -6491,13 +6692,13 @@
         <v>362</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>140</v>
       </c>
@@ -6515,7 +6716,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -6525,7 +6726,7 @@
       <c r="E20" s="60"/>
       <c r="F20" s="60"/>
     </row>
-    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -6539,13 +6740,13 @@
         <v>326</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>149</v>
       </c>
@@ -6559,13 +6760,13 @@
         <v>363</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
@@ -6579,13 +6780,13 @@
         <v>364</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>140</v>
       </c>
@@ -6603,7 +6804,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
@@ -6613,7 +6814,7 @@
       <c r="E25" s="60"/>
       <c r="F25" s="60"/>
     </row>
-    <row r="26" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>110</v>
       </c>
@@ -6627,18 +6828,18 @@
         <v>365</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="13">
-        <v>2422</v>
+        <v>22</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>269</v>
@@ -6647,13 +6848,13 @@
         <v>366</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -6663,17 +6864,17 @@
       <c r="C28" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="14" t="s">
         <v>367</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>21</v>
       </c>
@@ -6687,13 +6888,13 @@
         <v>289</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>140</v>
       </c>
@@ -6711,7 +6912,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
@@ -6721,7 +6922,7 @@
       <c r="E31" s="60"/>
       <c r="F31" s="60"/>
     </row>
-    <row r="32" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>122</v>
       </c>
@@ -6735,10 +6936,10 @@
         <v>363</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -6755,10 +6956,10 @@
         <v>363</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -6775,10 +6976,10 @@
         <v>300</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -6795,10 +6996,10 @@
         <v>304</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6806,7 +7007,7 @@
         <v>140</v>
       </c>
       <c r="B36" s="13"/>
-      <c r="C36" s="28">
+      <c r="C36" s="78">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="D36" s="46">
@@ -6843,10 +7044,10 @@
         <v>326</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6863,10 +7064,10 @@
         <v>368</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6883,10 +7084,10 @@
         <v>307</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6897,7 +7098,7 @@
       <c r="C41" s="28">
         <v>0.12</v>
       </c>
-      <c r="D41" s="72">
+      <c r="D41" s="67">
         <v>0.26</v>
       </c>
       <c r="E41" s="28">
@@ -6931,10 +7132,10 @@
         <v>297</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6951,10 +7152,10 @@
         <v>366</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6962,10 +7163,10 @@
         <v>140</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="75">
+      <c r="C45" s="28">
         <v>0.75</v>
       </c>
-      <c r="D45" s="76">
+      <c r="D45" s="70">
         <v>0.1</v>
       </c>
       <c r="E45" s="28">
@@ -6999,10 +7200,10 @@
         <v>369</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -7019,10 +7220,10 @@
         <v>326</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -7039,10 +7240,10 @@
         <v>370</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7087,10 +7288,10 @@
         <v>371</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7107,10 +7308,10 @@
         <v>363</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7155,10 +7356,10 @@
         <v>289</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7175,10 +7376,10 @@
         <v>363</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7195,10 +7396,10 @@
         <v>326</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7215,10 +7416,10 @@
         <v>372</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7235,10 +7436,10 @@
         <v>317</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7255,10 +7456,10 @@
         <v>373</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7275,10 +7476,10 @@
         <v>374</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7323,10 +7524,10 @@
         <v>375</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F65" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7343,10 +7544,10 @@
         <v>376</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F66" s="28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7401,10 +7602,10 @@
         <v>377</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F70" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -7421,10 +7622,10 @@
         <v>363</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7469,10 +7670,10 @@
         <v>289</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -7489,10 +7690,10 @@
         <v>378</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -7537,10 +7738,10 @@
         <v>379</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -7557,10 +7758,10 @@
         <v>363</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7601,8 +7802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962561A6-620C-FF49-A044-E467A34D0B13}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7613,14 +7814,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="73" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -7643,7 +7844,7 @@
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="24" t="s">
-        <v>246</v>
+        <v>718</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>248</v>
@@ -7679,13 +7880,13 @@
         <v>274</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -7696,16 +7897,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -7716,16 +7917,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -7736,16 +7937,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -7753,7 +7954,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="75">
+      <c r="C9" s="28">
         <v>0.31</v>
       </c>
       <c r="D9" s="32">
@@ -7771,10 +7972,10 @@
         <v>282</v>
       </c>
       <c r="B10" s="37"/>
-      <c r="C10" s="67"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="37"/>
       <c r="E10" s="60"/>
-      <c r="F10" s="67"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -7787,13 +7988,13 @@
         <v>274</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -7804,27 +8005,27 @@
         <v>18</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="64" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="75">
+      <c r="C13" s="28">
         <v>0.11</v>
       </c>
-      <c r="D13" s="74">
+      <c r="D13" s="69">
         <v>0.33</v>
       </c>
       <c r="E13" s="28">
@@ -7855,13 +8056,13 @@
         <v>249</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7872,16 +8073,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>286</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7920,16 +8121,16 @@
         <v>26</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7940,16 +8141,16 @@
         <v>36</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7960,16 +8161,16 @@
         <v>1</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8008,16 +8209,16 @@
         <v>4</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>317</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8028,16 +8229,16 @@
         <v>18</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8050,14 +8251,14 @@
       <c r="C26" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="14" t="s">
         <v>325</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8068,16 +8269,16 @@
         <v>11</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>326</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8088,16 +8289,16 @@
         <v>5</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8105,7 +8306,7 @@
         <v>140</v>
       </c>
       <c r="B29" s="28"/>
-      <c r="C29" s="75">
+      <c r="C29" s="28">
         <v>0.72</v>
       </c>
       <c r="D29" s="46">
@@ -8139,13 +8340,13 @@
         <v>249</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8156,16 +8357,16 @@
         <v>17</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>289</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8179,13 +8380,13 @@
         <v>249</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8196,16 +8397,16 @@
         <v>6</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8247,13 +8448,13 @@
         <v>249</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -8264,16 +8465,16 @@
         <v>34</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>366</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.25">
@@ -8284,16 +8485,16 @@
         <v>5</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8304,7 +8505,7 @@
       <c r="C40" s="28">
         <v>0.46</v>
       </c>
-      <c r="D40" s="72">
+      <c r="D40" s="67">
         <v>0.97</v>
       </c>
       <c r="E40" s="46">
@@ -8332,16 +8533,16 @@
         <v>10</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8355,13 +8556,13 @@
         <v>249</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8372,7 +8573,7 @@
       <c r="C44" s="62">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="D44" s="76">
+      <c r="D44" s="70">
         <v>0.53</v>
       </c>
       <c r="E44" s="28">
@@ -8403,13 +8604,13 @@
         <v>249</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8423,13 +8624,13 @@
         <v>262</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8440,16 +8641,16 @@
         <v>11</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8488,16 +8689,16 @@
         <v>18</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8511,13 +8712,13 @@
         <v>277</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8556,16 +8757,16 @@
         <v>1</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8576,16 +8777,16 @@
         <v>27</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>289</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8596,16 +8797,16 @@
         <v>14</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8616,16 +8817,16 @@
         <v>8</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8636,16 +8837,16 @@
         <v>4</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8656,16 +8857,16 @@
         <v>2</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E60" s="28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8676,16 +8877,16 @@
         <v>7</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E61" s="28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8727,13 +8928,13 @@
         <v>249</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F64" s="28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8744,16 +8945,16 @@
         <v>1</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>358</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F65" s="28" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8761,7 +8962,7 @@
         <v>140</v>
       </c>
       <c r="B66" s="13"/>
-      <c r="C66" s="75">
+      <c r="C66" s="28">
         <v>0.33</v>
       </c>
       <c r="D66" s="28">
@@ -8802,16 +9003,16 @@
         <v>39</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D69" s="28" t="s">
         <v>289</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8822,16 +9023,16 @@
         <v>23</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F70" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -8873,13 +9074,13 @@
         <v>331</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -8893,13 +9094,13 @@
         <v>249</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -8941,13 +9142,13 @@
         <v>262</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -8958,16 +9159,16 @@
         <v>28</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>366</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9006,8 +9207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A83C731-2B95-FF4F-8B89-62FFA0834579}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9020,14 +9221,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="73" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -9050,7 +9251,7 @@
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="24" t="s">
-        <v>381</v>
+        <v>718</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>248</v>
@@ -9089,10 +9290,10 @@
         <v>326</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -9103,16 +9304,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -9123,16 +9324,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>363</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -9143,16 +9344,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>326</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -9178,10 +9379,10 @@
         <v>282</v>
       </c>
       <c r="B10" s="37"/>
-      <c r="C10" s="67"/>
+      <c r="C10" s="63"/>
       <c r="D10" s="37"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -9197,10 +9398,10 @@
         <v>326</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -9211,27 +9412,27 @@
         <v>18</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>363</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="64" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="62">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D13" s="71">
+      <c r="D13" s="66">
         <v>0.48</v>
       </c>
       <c r="E13" s="28">
@@ -9259,16 +9460,16 @@
         <v>43</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>367</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9279,16 +9480,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9327,16 +9528,16 @@
         <v>26</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9347,16 +9548,16 @@
         <v>36</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9395,16 +9596,16 @@
         <v>4</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9418,13 +9619,13 @@
         <v>331</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9437,14 +9638,14 @@
       <c r="C25" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="D25" s="69" t="s">
+      <c r="D25" s="14" t="s">
         <v>326</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9455,16 +9656,16 @@
         <v>11</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9472,7 +9673,7 @@
         <v>140</v>
       </c>
       <c r="B27" s="28"/>
-      <c r="C27" s="62">
+      <c r="C27" s="75">
         <v>0.78</v>
       </c>
       <c r="D27" s="46">
@@ -9503,16 +9704,16 @@
         <v>17</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>326</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9526,13 +9727,13 @@
         <v>273</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9549,10 +9750,10 @@
         <v>326</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -9563,16 +9764,16 @@
         <v>6</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9611,16 +9812,16 @@
         <v>24</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>318</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -9637,10 +9838,10 @@
         <v>377</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -9654,13 +9855,13 @@
         <v>333</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9671,7 +9872,7 @@
       <c r="C38" s="28">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D38" s="72">
+      <c r="D38" s="67">
         <v>0.68</v>
       </c>
       <c r="E38" s="28">
@@ -9699,16 +9900,16 @@
         <v>10</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9725,10 +9926,10 @@
         <v>326</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9736,10 +9937,10 @@
         <v>140</v>
       </c>
       <c r="B42" s="13"/>
-      <c r="C42" s="62">
+      <c r="C42" s="75">
         <v>0.82</v>
       </c>
-      <c r="D42" s="74">
+      <c r="D42" s="69">
         <v>0.34</v>
       </c>
       <c r="E42" s="28">
@@ -9773,10 +9974,10 @@
         <v>326</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9787,16 +9988,16 @@
         <v>26</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9807,16 +10008,16 @@
         <v>11</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>363</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9858,13 +10059,13 @@
         <v>333</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9881,10 +10082,10 @@
         <v>363</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9923,16 +10124,16 @@
         <v>1</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D53" s="13" t="s">
         <v>358</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9949,10 +10150,10 @@
         <v>318</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9963,16 +10164,16 @@
         <v>14</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>318</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9983,16 +10184,16 @@
         <v>8</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>286</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10003,16 +10204,16 @@
         <v>4</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10023,16 +10224,16 @@
         <v>2</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10046,13 +10247,13 @@
         <v>333</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10097,10 +10298,10 @@
         <v>326</v>
       </c>
       <c r="E62" s="28" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10111,16 +10312,16 @@
         <v>1</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>358</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10128,7 +10329,7 @@
         <v>140</v>
       </c>
       <c r="B64" s="13"/>
-      <c r="C64" s="62">
+      <c r="C64" s="75">
         <v>0.66</v>
       </c>
       <c r="D64" s="46">
@@ -10175,10 +10376,10 @@
         <v>378</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F67" s="28" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10189,16 +10390,16 @@
         <v>23</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D68" s="28" t="s">
         <v>326</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10243,10 +10444,10 @@
         <v>289</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -10263,10 +10464,10 @@
         <v>326</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -10311,10 +10512,10 @@
         <v>326</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -10325,16 +10526,16 @@
         <v>28</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -10371,6 +10572,89 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33C5496-F7B3-B34C-8942-3D3A56FFBD47}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="6" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57" t="s">
+        <v>707</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>708</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>709</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>710</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4">
+        <v>3946.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="B6" ca="1">Demo_tri2_weekend!J10:N17</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>715</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8538B0B0-23EC-F344-B781-ACBD2A27A8BA}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added final tables, incorporated some (not yet all) of Erica's chapter 3 edits, finalized formatting, and added supplementary tables
</commit_message>
<xml_diff>
--- a/Dissertation Chapters/Chapter 3/PRESS_Chapter3_tables.xlsx
+++ b/Dissertation Chapters/Chapter 3/PRESS_Chapter3_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mollyec/Documents/GitHub/Developmental-Obesity/Dissertation Chapters/Chapter 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC67D8E0-4D94-F345-8AE5-F1D5C89B7275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5960FF3-963E-A443-8C7B-583DFB5FB933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="28240" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{5531AC36-D13B-7248-9642-950AE3589228}"/>
+    <workbookView xWindow="-25000" yWindow="1920" windowWidth="25600" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{5531AC36-D13B-7248-9642-950AE3589228}"/>
   </bookViews>
   <sheets>
     <sheet name=" Base Demographics" sheetId="1" r:id="rId1"/>
@@ -3357,7 +3357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3791,6 +3791,33 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3824,39 +3851,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3876,7 +3881,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4164,7 +4169,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4185,10 +4190,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="166" t="s">
         <v>870</v>
       </c>
-      <c r="B1" s="158"/>
+      <c r="B1" s="167"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4793,8 +4798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC7E06F-17C5-3049-BDAA-1EF80623DF9F}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4806,16 +4811,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="176" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
       <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -5419,18 +5424,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="173" t="s">
         <v>979</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-    </row>
-    <row r="2" spans="1:9" s="178" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="179"/>
-      <c r="B2" s="179"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="179"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="177"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="129"/>
       <c r="F2" s="129"/>
       <c r="G2" s="129"/>
@@ -5438,26 +5443,26 @@
       <c r="I2" s="129"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="168"/>
-      <c r="B3" s="168" t="s">
+      <c r="A3" s="157"/>
+      <c r="B3" s="157" t="s">
         <v>604</v>
       </c>
-      <c r="C3" s="175" t="s">
+      <c r="C3" s="163" t="s">
         <v>622</v>
       </c>
-      <c r="D3" s="175" t="s">
+      <c r="D3" s="163" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="158" t="s">
         <v>968</v>
       </c>
-      <c r="B4" s="170"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="159"/>
+      <c r="C4" s="164" t="s">
         <v>605</v>
       </c>
-      <c r="D4" s="176" t="s">
+      <c r="D4" s="164" t="s">
         <v>605</v>
       </c>
     </row>
@@ -5561,19 +5566,19 @@
       <c r="C12" s="155">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D12" s="173">
+      <c r="D12" s="162">
         <v>0.89</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="160" t="s">
         <v>971</v>
       </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="177" t="s">
+      <c r="B13" s="160"/>
+      <c r="C13" s="165" t="s">
         <v>605</v>
       </c>
-      <c r="D13" s="177" t="s">
+      <c r="D13" s="165" t="s">
         <v>605</v>
       </c>
     </row>
@@ -5670,10 +5675,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="172" t="s">
+      <c r="A21" s="161" t="s">
         <v>960</v>
       </c>
-      <c r="B21" s="172"/>
+      <c r="B21" s="161"/>
       <c r="C21" s="118">
         <v>0.85</v>
       </c>
@@ -5682,7 +5687,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="174" t="s">
+      <c r="A23" s="131" t="s">
         <v>967</v>
       </c>
     </row>
@@ -5710,14 +5715,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="168" t="s">
         <v>863</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
     </row>
     <row r="2" spans="1:6" ht="52" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -7136,14 +7141,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="170" t="s">
         <v>862</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="84"/>
@@ -8562,14 +8567,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="168" t="s">
         <v>864</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
     </row>
     <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -9969,14 +9974,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="168" t="s">
         <v>865</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
     </row>
     <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -11337,12 +11342,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="55" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="172" t="s">
         <v>871</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
     </row>
@@ -12464,12 +12469,12 @@
       <c r="E85"/>
     </row>
     <row r="86" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="164" t="s">
+      <c r="A86" s="173" t="s">
         <v>959</v>
       </c>
-      <c r="B86" s="164"/>
-      <c r="C86" s="164"/>
-      <c r="D86" s="164"/>
+      <c r="B86" s="173"/>
+      <c r="C86" s="173"/>
+      <c r="D86" s="173"/>
       <c r="E86"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -13059,32 +13064,32 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:I5"/>
+      <selection activeCell="A28" sqref="A1:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="28" customWidth="1"/>
-    <col min="3" max="9" width="19.83203125" style="28" customWidth="1"/>
+    <col min="3" max="9" width="22.83203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="174" t="s">
         <v>963</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="130"/>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="178" t="s">
         <v>604</v>
       </c>
       <c r="C2" s="130" t="s">
@@ -13113,7 +13118,7 @@
       <c r="A3" s="133" t="s">
         <v>610</v>
       </c>
-      <c r="B3" s="134"/>
+      <c r="B3" s="135"/>
       <c r="C3" s="134" t="s">
         <v>605</v>
       </c>
@@ -13140,7 +13145,7 @@
       <c r="A4" s="129" t="s">
         <v>611</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="151" t="s">
         <v>623</v>
       </c>
       <c r="C4" s="151" t="s">
@@ -13169,7 +13174,7 @@
       <c r="A5" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B5" s="129"/>
+      <c r="B5" s="151"/>
       <c r="C5" s="151">
         <v>0.18</v>
       </c>
@@ -13196,7 +13201,7 @@
       <c r="A6" s="129" t="s">
         <v>612</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="151" t="s">
         <v>680</v>
       </c>
       <c r="C6" s="151" t="s">
@@ -13225,7 +13230,7 @@
       <c r="A7" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B7" s="129"/>
+      <c r="B7" s="151"/>
       <c r="C7" s="151">
         <v>0.19</v>
       </c>
@@ -13252,7 +13257,7 @@
       <c r="A8" s="129" t="s">
         <v>613</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="154" t="s">
         <v>682</v>
       </c>
       <c r="C8" s="154" t="s">
@@ -13281,7 +13286,7 @@
       <c r="A9" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B9" s="131"/>
+      <c r="B9" s="154"/>
       <c r="C9" s="154">
         <v>9.4E-2</v>
       </c>
@@ -13308,7 +13313,7 @@
       <c r="A10" s="129" t="s">
         <v>614</v>
       </c>
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="151" t="s">
         <v>712</v>
       </c>
       <c r="C10" s="151" t="s">
@@ -13337,7 +13342,7 @@
       <c r="A11" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B11" s="129"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="151">
         <v>0.87</v>
       </c>
@@ -13364,7 +13369,7 @@
       <c r="A12" s="133" t="s">
         <v>615</v>
       </c>
-      <c r="B12" s="133"/>
+      <c r="B12" s="179"/>
       <c r="C12" s="134" t="s">
         <v>605</v>
       </c>
@@ -13391,7 +13396,7 @@
       <c r="A13" s="129" t="s">
         <v>611</v>
       </c>
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="151" t="s">
         <v>679</v>
       </c>
       <c r="C13" s="151" t="s">
@@ -13420,7 +13425,7 @@
       <c r="A14" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B14" s="129"/>
+      <c r="B14" s="151"/>
       <c r="C14" s="151">
         <v>0.41</v>
       </c>
@@ -13447,7 +13452,7 @@
       <c r="A15" s="129" t="s">
         <v>612</v>
       </c>
-      <c r="B15" s="129" t="s">
+      <c r="B15" s="151" t="s">
         <v>664</v>
       </c>
       <c r="C15" s="151" t="s">
@@ -13476,7 +13481,7 @@
       <c r="A16" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B16" s="129"/>
+      <c r="B16" s="151"/>
       <c r="C16" s="151">
         <v>6.0299999999999999E-2</v>
       </c>
@@ -13503,7 +13508,7 @@
       <c r="A17" s="129" t="s">
         <v>613</v>
       </c>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="151" t="s">
         <v>697</v>
       </c>
       <c r="C17" s="151" t="s">
@@ -13532,7 +13537,7 @@
       <c r="A18" s="129" t="s">
         <v>960</v>
       </c>
-      <c r="B18" s="129"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="152">
         <v>1.1E-4</v>
       </c>
@@ -13559,7 +13564,7 @@
       <c r="A19" s="129" t="s">
         <v>614</v>
       </c>
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="151" t="s">
         <v>727</v>
       </c>
       <c r="C19" s="151" t="s">
@@ -13588,7 +13593,7 @@
       <c r="A20" s="132" t="s">
         <v>960</v>
       </c>
-      <c r="B20" s="132"/>
+      <c r="B20" s="156"/>
       <c r="C20" s="155">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -13728,55 +13733,54 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection sqref="A1:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="28" customWidth="1"/>
-    <col min="3" max="4" width="21.5" style="28" customWidth="1"/>
-    <col min="5" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="28" customWidth="1"/>
+    <col min="3" max="4" width="21.6640625" style="28" customWidth="1"/>
+    <col min="5" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="174" t="s">
         <v>964</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="130"/>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="178" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="178" t="s">
         <v>622</v>
       </c>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="178" t="s">
         <v>600</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="178" t="s">
         <v>601</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="178" t="s">
         <v>602</v>
       </c>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="178" t="s">
         <v>603</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="178" t="s">
         <v>620</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="178" t="s">
         <v>621</v>
       </c>
     </row>
@@ -14286,81 +14290,105 @@
       <c r="A21" s="94" t="s">
         <v>962</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="180"/>
+      <c r="H21" s="180"/>
+      <c r="I21" s="180"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="94" t="s">
         <v>616</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
+      <c r="B22" s="180"/>
+      <c r="C22" s="180"/>
+      <c r="D22" s="180"/>
+      <c r="E22" s="180"/>
+      <c r="F22" s="180"/>
+      <c r="G22" s="180"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="180"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="94" t="s">
         <v>607</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
+      <c r="B23" s="180"/>
+      <c r="C23" s="180"/>
+      <c r="D23" s="180"/>
+      <c r="E23" s="180"/>
+      <c r="F23" s="180"/>
+      <c r="G23" s="180"/>
+      <c r="H23" s="180"/>
+      <c r="I23" s="180"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="94" t="s">
         <v>608</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
+      <c r="B24" s="180"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="94" t="s">
         <v>609</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+      <c r="B25" s="180"/>
+      <c r="C25" s="180"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="180"/>
+      <c r="F25" s="180"/>
+      <c r="G25" s="180"/>
+      <c r="H25" s="180"/>
+      <c r="I25" s="180"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="94" t="s">
         <v>617</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
+      <c r="B26" s="180"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
+      <c r="E26" s="180"/>
+      <c r="F26" s="180"/>
+      <c r="G26" s="180"/>
+      <c r="H26" s="180"/>
+      <c r="I26" s="180"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="94" t="s">
         <v>618</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+      <c r="B27" s="180"/>
+      <c r="C27" s="180"/>
+      <c r="D27" s="180"/>
+      <c r="E27" s="180"/>
+      <c r="F27" s="180"/>
+      <c r="G27" s="180"/>
+      <c r="H27" s="180"/>
+      <c r="I27" s="180"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="94" t="s">
         <v>619</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
+      <c r="B28" s="180"/>
+      <c r="C28" s="180"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="180"/>
+      <c r="F28" s="180"/>
+      <c r="G28" s="180"/>
+      <c r="H28" s="180"/>
+      <c r="I28" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14374,8 +14402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD4CBF1-CDE4-4F46-BE6F-28F64D99A949}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14388,16 +14416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="175" t="s">
         <v>965</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
       <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>